<commit_message>
database nya di dir database kang
</commit_message>
<xml_diff>
--- a/excel/import_data.xlsx
+++ b/excel/import_data.xlsx
@@ -101,12 +101,6 @@
     <t>ID_SEMESTER</t>
   </si>
   <si>
-    <t>Juned</t>
-  </si>
-  <si>
-    <t>juned@gmail.com</t>
-  </si>
-  <si>
     <t>adjaksdju38</t>
   </si>
   <si>
@@ -135,6 +129,12 @@
   </si>
   <si>
     <t>PMB_lamah</t>
+  </si>
+  <si>
+    <t>Casgoni</t>
+  </si>
+  <si>
+    <t>casgoni@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Y2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,19 +603,19 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>31231</v>
+        <v>9931231</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" t="s">
         <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
@@ -627,22 +627,22 @@
         <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J2">
         <v>338</v>
       </c>
       <c r="K2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L2" s="2">
         <v>33604</v>
       </c>
       <c r="M2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="O2">
         <v>383838</v>
@@ -651,16 +651,16 @@
         <v>3928183</v>
       </c>
       <c r="Q2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" t="s">
         <v>34</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>35</v>
-      </c>
-      <c r="S2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" t="s">
-        <v>37</v>
       </c>
       <c r="U2">
         <v>1</v>
@@ -682,6 +682,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>